<commit_message>
Defocus fix and partial fix to LIONbeam
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/DefocusQuadrupole.xlsx
+++ b/21-Spreads4Tests/DefocusQuadrupole.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARA_Beamline/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longkr/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2AF286-2125-9543-BEAE-EF8DCE336FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAFB5DF-26D3-EB45-BE86-A2C9E6976077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="640" windowWidth="28040" windowHeight="17440" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="19400" yWindow="0" windowWidth="19000" windowHeight="21600" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>p</t>
   </si>
@@ -134,12 +134,43 @@
   <si>
     <t>s/m</t>
   </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>p</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MeV/c</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -169,6 +200,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -543,7 +580,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,7 +900,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="E15" sqref="E15:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,7 +919,7 @@
       <c r="E1" s="28"/>
       <c r="F1" s="29"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="20" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="4" t="s">
         <v>5</v>
@@ -891,12 +930,21 @@
         <v>6</v>
       </c>
       <c r="F2" s="5"/>
+      <c r="H2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="12">
+        <v>938.27208815999995</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1">
         <v>20</v>
       </c>
       <c r="C3" t="s">
@@ -922,16 +970,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9">
-        <f>I5*B3/1000</f>
-        <v>6.6712819039630403E-2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="30"/>
       <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
@@ -944,7 +984,7 @@
       <c r="H4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4">
         <f>1/I3</f>
         <v>3.3356409519815204E-9</v>
       </c>
@@ -953,6 +993,16 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <f>SQRT( (I2+B3)^2 - I2^2)</f>
+        <v>194.75852619692921</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
       <c r="D5" s="13"/>
       <c r="F5" s="7"/>
       <c r="H5" s="8" t="s">
@@ -967,12 +1017,22 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9">
+        <f>I5*B5/1000</f>
+        <v>0.64964451573004278</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>3</v>
+      </c>
       <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E6">
-        <f>E4/B4</f>
-        <v>1498.9622900000002</v>
+        <f>E4/B6</f>
+        <v>153.93033817521612</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>12</v>
@@ -984,7 +1044,7 @@
       </c>
       <c r="E7">
         <f>SQRT(E6)</f>
-        <v>38.716434365783222</v>
+        <v>12.406866573604155</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>14</v>
@@ -996,7 +1056,7 @@
       </c>
       <c r="E8" s="9">
         <f>E7*E3</f>
-        <v>3.8716434365783226</v>
+        <v>1.2406866573604156</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -1006,11 +1066,11 @@
       </c>
       <c r="B10" s="14">
         <f>COSH(E8)</f>
-        <v>24.021032624407752</v>
+        <v>1.8735863401848911</v>
       </c>
       <c r="C10" s="15">
         <f>SINH(E8)/E7</f>
-        <v>0.61989718060008403</v>
+        <v>0.12770353839489526</v>
       </c>
       <c r="D10" s="15">
         <v>0</v>
@@ -1022,11 +1082,11 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="17">
         <f>SINH(E8)*E7</f>
-        <v>929.20249739684562</v>
+        <v>19.657448851297922</v>
       </c>
       <c r="C11" s="18">
         <f>COSH(E8)</f>
-        <v>24.021032624407752</v>
+        <v>1.8735863401848911</v>
       </c>
       <c r="D11" s="18">
         <v>0</v>
@@ -1044,11 +1104,11 @@
       </c>
       <c r="D12" s="18">
         <f>COS(E8)</f>
-        <v>-0.74514053575099048</v>
+        <v>0.32414677837477512</v>
       </c>
       <c r="E12" s="19">
         <f>SIN(E8)/E7</f>
-        <v>-1.7225436361885331E-2</v>
+        <v>7.6248647844430473E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1060,11 +1120,11 @@
       </c>
       <c r="D13" s="21">
         <f>-SIN(E8)*E7</f>
-        <v>25.820279535260905</v>
+        <v>-11.736980148096146</v>
       </c>
       <c r="E13" s="22">
         <f>COS(E8)</f>
-        <v>-0.74514053575099048</v>
+        <v>0.32414677837477512</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1079,14 +1139,14 @@
       </c>
       <c r="E15" s="24">
         <f t="array" ref="E15:E18">MMULT(B10:E13,B15:B18)</f>
-        <v>12.072506030263884</v>
+        <v>0.94956352393193511</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H15" s="24">
         <f>B$15*B10+B$16*C10+B$17*D10+B$18*E10</f>
-        <v>12.072506030263884</v>
+        <v>0.94956352393193511</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1094,11 +1154,11 @@
         <v>0.1</v>
       </c>
       <c r="E16" s="25">
-        <v>467.0033519608636</v>
+        <v>10.01608305966745</v>
       </c>
       <c r="H16" s="25">
         <f t="shared" ref="H16:H17" si="0">B$15*B11+B$16*C11+B$17*D11+B$18*E11</f>
-        <v>467.0033519608636</v>
+        <v>10.01608305966745</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
@@ -1106,11 +1166,11 @@
         <v>-0.3</v>
       </c>
       <c r="E17" s="25">
-        <v>0.22698724799767422</v>
+        <v>-0.11249376308131863</v>
       </c>
       <c r="H17" s="25">
         <f t="shared" si="0"/>
-        <v>0.22698724799767422</v>
+        <v>-0.11249376308131863</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -1118,11 +1178,11 @@
         <v>-0.2</v>
       </c>
       <c r="E18" s="26">
-        <v>-7.5970557534280729</v>
+        <v>3.456264688753889</v>
       </c>
       <c r="H18" s="26">
         <f>B$15*B13+B$16*C13+B$17*D13+B$18*E13</f>
-        <v>-7.5970557534280729</v>
+        <v>3.456264688753889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checks and updates to make self consistent
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/DefocusQuadrupole.xlsx
+++ b/21-Spreads4Tests/DefocusQuadrupole.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47AF719-9C7F-E54D-A82F-29C89061DA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E005FC1-8D9D-6844-B340-9F6701CD4292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15080" windowHeight="18900" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="27720" yWindow="500" windowWidth="29400" windowHeight="23120" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>p</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>Diff</t>
+  </si>
+  <si>
+    <t>Focus quad test sheet: no reference particle</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -540,51 +543,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="dotted">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -616,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -641,6 +599,51 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -653,11 +656,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -667,11 +665,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -681,46 +674,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,9 +692,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -779,7 +732,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -885,7 +838,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1027,7 +980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1035,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,45 +1000,62 @@
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38"/>
+      <c r="L1" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="38"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2"/>
-      <c r="H2" s="29" t="s">
+      <c r="F2" s="17"/>
+      <c r="H2" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-    </row>
-    <row r="3" spans="1:10" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
+      <c r="L2" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="40"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="17"/>
+    </row>
+    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="19">
         <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E3">
@@ -1094,8 +1064,7 @@
       <c r="F3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G3"/>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="20" t="s">
         <v>5</v>
       </c>
       <c r="I3">
@@ -1104,19 +1073,37 @@
       <c r="J3" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" s="21" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="L3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="19">
+        <v>20</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>0.1</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="19">
         <f>I10+B3</f>
         <v>958.27208815999995</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E4">
@@ -1125,8 +1112,7 @@
       <c r="F4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G4"/>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="20" t="s">
         <v>27</v>
       </c>
       <c r="I4">
@@ -1136,12 +1122,31 @@
       <c r="J4" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="L4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="19">
+        <f>I10+M3</f>
+        <v>958.27208815999995</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="19">
         <f>SQRT(B4^2 -I10^ 2)</f>
         <v>194.75852619692921</v>
       </c>
@@ -1149,15 +1154,27 @@
         <v>1</v>
       </c>
       <c r="D5" s="7"/>
-      <c r="E5" s="35"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="9"/>
-      <c r="G5"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
-    </row>
-    <row r="6" spans="1:10" s="21" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="24"/>
+      <c r="L5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="19">
+        <f>SQRT(M4^2 -I10^ 2)</f>
+        <v>194.75852619692921</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B6">
@@ -1165,7 +1182,7 @@
         <v>0.20757148022900346</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="26" t="s">
         <v>2</v>
       </c>
       <c r="E6">
@@ -1173,13 +1190,27 @@
         <v>0.64964451573004278</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6"/>
       <c r="H6" s="12"/>
-      <c r="I6"/>
       <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" s="21" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="L6" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6">
+        <f>M5/I10</f>
+        <v>0.20757148022900346</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <f>M12*I13/1000</f>
+        <v>1.6137238800416533</v>
+      </c>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B7">
@@ -1187,7 +1218,7 @@
         <v>0.20323927682260837</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="20" t="s">
         <v>38</v>
       </c>
       <c r="E7">
@@ -1197,8 +1228,7 @@
       <c r="F7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G7"/>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="20" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="1">
@@ -1208,8 +1238,26 @@
       <c r="J7" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <f>M5/M4</f>
+        <v>0.20323927682260837</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7">
+        <f>P4/P6</f>
+        <v>61.968470093792504</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
@@ -1217,38 +1265,39 @@
         <v>1</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="41"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
-      <c r="G8"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="42"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="28"/>
       <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9"/>
-      <c r="C9"/>
+      <c r="L8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="9"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D9" s="1"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9" s="40"/>
+      <c r="H9" s="26"/>
       <c r="I9" s="13"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:10" s="21" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+    </row>
+    <row r="10" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="23" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
-      <c r="G10"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
       <c r="H10" s="10" t="s">
         <v>20</v>
       </c>
@@ -1258,8 +1307,18 @@
       <c r="J10" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="41"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>33</v>
       </c>
@@ -1267,8 +1326,7 @@
         <f>B4+B5*B30</f>
         <v>1055.6513512584645</v>
       </c>
-      <c r="C11"/>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="29" t="s">
         <v>34</v>
       </c>
       <c r="E11">
@@ -1276,7 +1334,6 @@
         <v>2.4840106257623371</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11"/>
       <c r="H11" s="10" t="s">
         <v>15</v>
       </c>
@@ -1286,17 +1343,31 @@
       <c r="J11" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" s="21" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="L11" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11">
+        <f>M4+M5*B30</f>
+        <v>1055.6513512584645</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="19">
         <f>SQRT(B11^2 -I10^ 2)</f>
         <v>483.78224853098436</v>
       </c>
-      <c r="C12"/>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="29" t="s">
         <v>35</v>
       </c>
       <c r="E12">
@@ -1306,7 +1377,6 @@
       <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G12"/>
       <c r="H12" s="5" t="s">
         <v>16</v>
       </c>
@@ -1317,12 +1387,29 @@
       <c r="J12" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="44"/>
-      <c r="B13"/>
+      <c r="L12" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="19">
+        <f>SQRT(M11^2 -I10^ 2)</f>
+        <v>483.78224853098436</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12">
+        <f>SQRT(P7/P11)</f>
+        <v>7.8720054683538239</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="30"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="29" t="s">
         <v>36</v>
       </c>
       <c r="E13">
@@ -1330,7 +1417,6 @@
         <v>0.78720054683538221</v>
       </c>
       <c r="F13" s="6"/>
-      <c r="G13"/>
       <c r="H13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1341,12 +1427,22 @@
       <c r="J13" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" s="21" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="45"/>
+      <c r="L13" s="30"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13">
+        <f>P12*P3</f>
+        <v>0.78720054683538243</v>
+      </c>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="31"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="27" t="s">
         <v>37</v>
       </c>
       <c r="E14" s="8">
@@ -1356,28 +1452,37 @@
       <c r="F14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="31"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="P14" s="8">
+        <f>P12*P11</f>
+        <v>7.8720054683538239</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>3</v>
       </c>
@@ -1401,9 +1506,32 @@
       <c r="G18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="46">
+      <c r="L18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" s="3">
+        <f>COSH(P13)</f>
+        <v>1.3261769198076012</v>
+      </c>
+      <c r="N18" s="4">
+        <f>SINH(P13)/P14</f>
+        <v>0.11065284834228896</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0</v>
+      </c>
+      <c r="P18" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B19" s="32">
         <f>SINH(E13)*E14</f>
         <v>17.032830365379439</v>
       </c>
@@ -1423,12 +1551,33 @@
       <c r="G19" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="1"/>
+      <c r="M19" s="32">
+        <f>SINH(P13)*P14</f>
+        <v>6.8569877232920904</v>
+      </c>
+      <c r="N19" s="9">
+        <f>COSH(P13)</f>
+        <v>1.3261769198076012</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B20" s="12">
         <v>0</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20">
         <v>0</v>
       </c>
       <c r="D20" s="3">
@@ -1445,15 +1594,36 @@
       <c r="G20" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="1"/>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="3">
+        <f>COS(P13)</f>
+        <v>0.70583115577702327</v>
+      </c>
+      <c r="P20" s="4">
+        <f>SIN(P13)/P14</f>
+        <v>8.9987248147529314E-2</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B21" s="12">
         <v>0</v>
       </c>
-      <c r="C21" s="20">
-        <v>0</v>
-      </c>
-      <c r="D21" s="46">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="32">
         <f>-SIN(E13)*E14</f>
         <v>-13.851767538806278</v>
       </c>
@@ -1467,8 +1637,29 @@
       <c r="G21" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="1"/>
+      <c r="M21" s="12">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="32">
+        <f>-SIN(P13)*P14</f>
+        <v>-5.5763720956528555</v>
+      </c>
+      <c r="P21" s="9">
+        <f>COS(P13)</f>
+        <v>0.70583115577702327</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B22" s="12">
         <v>0</v>
       </c>
@@ -1488,9 +1679,29 @@
         <f>E3/B6^2</f>
         <v>2.3209438578128516</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="46">
+      <c r="L22" s="1"/>
+      <c r="M22" s="12">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>1</v>
+      </c>
+      <c r="R22" s="4">
+        <f>P3/M6^2</f>
+        <v>2.3209438578128516</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B23" s="32">
         <v>0</v>
       </c>
       <c r="C23" s="8">
@@ -1502,124 +1713,258 @@
       <c r="E23" s="8">
         <v>0</v>
       </c>
-      <c r="F23" s="46">
+      <c r="F23" s="32">
         <v>0</v>
       </c>
       <c r="G23" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="1"/>
+      <c r="M23" s="32">
+        <v>0</v>
+      </c>
+      <c r="N23" s="8">
+        <v>0</v>
+      </c>
+      <c r="O23" s="8">
+        <v>0</v>
+      </c>
+      <c r="P23" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="32">
+        <v>0</v>
+      </c>
+      <c r="R23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="33">
         <v>0.5</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="14">
-        <f t="array" ref="E25:E30">MMULT(B18:G23,B25:B30)</f>
+      <c r="D25" s="33">
+        <f t="array" ref="D25:D30">MMULT(B18:G23,B25:B30)</f>
         <v>0.66754306437266542</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="47">
+      <c r="F25" s="33">
         <f>B$25*B18+B$26*C18+B$27*D18+B$28*E18+B$29*F18+B$30*G18</f>
         <v>0.66754306437266542</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="G25" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="K25" s="14">
-        <f>E25-H25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="15">
+      <c r="H25" s="33">
+        <f>D25-F25</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="33">
+        <f>B25</f>
+        <v>0.5</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="33">
+        <f t="array" ref="O25:O30">MMULT(M18:R23,M25:M30)</f>
+        <v>0.67415374473802947</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25" s="33">
+        <f>M$25*M18+M$26*N18+M$27*O18+M$28*P18+M$29*Q18+M$30*R18</f>
+        <v>0.67415374473802947</v>
+      </c>
+      <c r="R25" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="S25" s="33">
+        <f t="shared" ref="S25:S30" si="0">O25-Q25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B26" s="34">
         <v>0.1</v>
       </c>
-      <c r="E26" s="15">
+      <c r="D26" s="34">
         <v>8.6490328746704801</v>
       </c>
-      <c r="H26" s="48">
-        <f t="shared" ref="H26:H30" si="0">B$25*B19+B$26*C19+B$27*D19+B$28*E19+B$29*F19+B$30*G19</f>
+      <c r="F26" s="34">
+        <f>B$25*B19+B$26*C19+B$27*D19+B$28*E19+B$29*F19+B$30*G19</f>
         <v>8.6490328746704801</v>
       </c>
-      <c r="K26" s="15">
-        <f t="shared" ref="K26:K30" si="1">E26-H26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="15">
+      <c r="H26" s="34">
+        <f>D26-F26</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="34">
+        <f t="shared" ref="M26:M30" si="1">B26</f>
+        <v>0.1</v>
+      </c>
+      <c r="O26" s="34">
+        <v>3.5611115536268052</v>
+      </c>
+      <c r="Q26" s="34">
+        <f t="shared" ref="Q26:Q30" si="2">M$25*M19+M$26*N19+M$27*O19+M$28*P19+M$29*Q19+M$30*R19</f>
+        <v>3.5611115536268052</v>
+      </c>
+      <c r="S26" s="34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B27" s="34">
         <v>-0.3</v>
       </c>
-      <c r="E27" s="15">
+      <c r="D27" s="34">
         <v>-0.21899466583232885</v>
       </c>
-      <c r="H27" s="48">
+      <c r="F27" s="34">
+        <f>B$25*B20+B$26*C20+B$27*D20+B$28*E20+B$29*F20+B$30*G20</f>
+        <v>-0.21899466583232885</v>
+      </c>
+      <c r="H27" s="34">
+        <f>D27-F27</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="34">
+        <f t="shared" si="1"/>
+        <v>-0.3</v>
+      </c>
+      <c r="O27" s="34">
+        <v>-0.22974679636261283</v>
+      </c>
+      <c r="Q27" s="34">
+        <f t="shared" si="2"/>
+        <v>-0.22974679636261283</v>
+      </c>
+      <c r="S27" s="34">
         <f t="shared" si="0"/>
-        <v>-0.21899466583232885</v>
-      </c>
-      <c r="K27" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B28" s="34">
+        <v>-0.2</v>
+      </c>
+      <c r="D28" s="34">
+        <v>4.0143640304864787</v>
+      </c>
+      <c r="F28" s="34">
+        <f>B$25*B21+B$26*C21+B$27*D21+B$28*E21+B$29*F21+B$30*G21</f>
+        <v>4.0143640304864787</v>
+      </c>
+      <c r="H28" s="34">
+        <f>D28-F28</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="15">
         <v>-0.2</v>
       </c>
-      <c r="E28" s="15">
-        <v>4.0143640304864787</v>
-      </c>
-      <c r="H28" s="48">
+      <c r="O28" s="34">
+        <v>1.5317453975404518</v>
+      </c>
+      <c r="Q28" s="34">
+        <f t="shared" si="2"/>
+        <v>1.5317453975404518</v>
+      </c>
+      <c r="S28" s="34">
         <f t="shared" si="0"/>
-        <v>4.0143640304864787</v>
-      </c>
-      <c r="K28" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B29" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="D29" s="34">
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="F29" s="34">
+        <f>B$25*B22+B$26*C22+B$27*D22+B$28*E22+B$29*F22+B$30*G22</f>
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="H29" s="34">
+        <f>D29-F29</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="1"/>
+      <c r="M29" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="15">
         <v>0.1</v>
       </c>
-      <c r="E29" s="15">
+      <c r="O29" s="34">
         <v>1.2604719289064259</v>
       </c>
-      <c r="H29" s="48">
+      <c r="Q29" s="34">
+        <f t="shared" si="2"/>
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="S29" s="34">
         <f t="shared" si="0"/>
-        <v>1.2604719289064259</v>
-      </c>
-      <c r="K29" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B30" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F30" s="35">
+        <f>B$25*B23+B$26*C23+B$27*D23+B$28*E23+B$29*F23+B$30*G23</f>
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="35">
+        <f>D30-F30</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="35">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B30" s="16">
         <v>0.5</v>
       </c>
-      <c r="E30" s="16">
+      <c r="O30" s="35">
         <v>0.5</v>
       </c>
-      <c r="H30" s="49">
+      <c r="Q30" s="35">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="S30" s="35">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="K30" s="16">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="H2:J2"/>

</xml_diff>

<commit_message>
Firszt QuadDoublet spread and completed quaddoublet test
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/DefocusQuadrupole.xlsx
+++ b/21-Spreads4Tests/DefocusQuadrupole.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E005FC1-8D9D-6844-B340-9F6701CD4292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7F2DA9-76B8-8A4B-A3C9-BBDF46AF6D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27720" yWindow="500" windowWidth="29400" windowHeight="23120" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
@@ -289,7 +289,7 @@
     <t>Diff</t>
   </si>
   <si>
-    <t>Focus quad test sheet: no reference particle</t>
+    <t>Deocus quad test sheet: no reference particle</t>
   </si>
 </sst>
 </file>
@@ -692,9 +692,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -732,7 +732,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -838,7 +838,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -980,7 +980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -991,7 +991,7 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L1" sqref="L1:S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1760,14 +1760,14 @@
         <v>13</v>
       </c>
       <c r="F25" s="33">
-        <f>B$25*B18+B$26*C18+B$27*D18+B$28*E18+B$29*F18+B$30*G18</f>
+        <f t="shared" ref="F25:F30" si="0">B$25*B18+B$26*C18+B$27*D18+B$28*E18+B$29*F18+B$30*G18</f>
         <v>0.66754306437266542</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>39</v>
       </c>
       <c r="H25" s="33">
-        <f>D25-F25</f>
+        <f t="shared" ref="H25:H30" si="1">D25-F25</f>
         <v>0</v>
       </c>
       <c r="L25" s="13" t="s">
@@ -1795,7 +1795,7 @@
         <v>39</v>
       </c>
       <c r="S25" s="33">
-        <f t="shared" ref="S25:S30" si="0">O25-Q25</f>
+        <f t="shared" ref="S25:S30" si="2">O25-Q25</f>
         <v>0</v>
       </c>
     </row>
@@ -1807,27 +1807,27 @@
         <v>8.6490328746704801</v>
       </c>
       <c r="F26" s="34">
-        <f>B$25*B19+B$26*C19+B$27*D19+B$28*E19+B$29*F19+B$30*G19</f>
+        <f t="shared" si="0"/>
         <v>8.6490328746704801</v>
       </c>
       <c r="H26" s="34">
-        <f>D26-F26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="34">
-        <f t="shared" ref="M26:M30" si="1">B26</f>
+        <f t="shared" ref="M26:M30" si="3">B26</f>
         <v>0.1</v>
       </c>
       <c r="O26" s="34">
         <v>3.5611115536268052</v>
       </c>
       <c r="Q26" s="34">
-        <f t="shared" ref="Q26:Q30" si="2">M$25*M19+M$26*N19+M$27*O19+M$28*P19+M$29*Q19+M$30*R19</f>
+        <f t="shared" ref="Q26:Q30" si="4">M$25*M19+M$26*N19+M$27*O19+M$28*P19+M$29*Q19+M$30*R19</f>
         <v>3.5611115536268052</v>
       </c>
       <c r="S26" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1839,27 +1839,27 @@
         <v>-0.21899466583232885</v>
       </c>
       <c r="F27" s="34">
-        <f>B$25*B20+B$26*C20+B$27*D20+B$28*E20+B$29*F20+B$30*G20</f>
+        <f t="shared" si="0"/>
         <v>-0.21899466583232885</v>
       </c>
       <c r="H27" s="34">
-        <f>D27-F27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L27" s="1"/>
       <c r="M27" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-0.3</v>
       </c>
       <c r="O27" s="34">
         <v>-0.22974679636261283</v>
       </c>
       <c r="Q27" s="34">
+        <f t="shared" si="4"/>
+        <v>-0.22974679636261283</v>
+      </c>
+      <c r="S27" s="34">
         <f t="shared" si="2"/>
-        <v>-0.22974679636261283</v>
-      </c>
-      <c r="S27" s="34">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1871,27 +1871,27 @@
         <v>4.0143640304864787</v>
       </c>
       <c r="F28" s="34">
-        <f>B$25*B21+B$26*C21+B$27*D21+B$28*E21+B$29*F21+B$30*G21</f>
+        <f t="shared" si="0"/>
         <v>4.0143640304864787</v>
       </c>
       <c r="H28" s="34">
-        <f>D28-F28</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-0.2</v>
       </c>
       <c r="O28" s="34">
         <v>1.5317453975404518</v>
       </c>
       <c r="Q28" s="34">
+        <f t="shared" si="4"/>
+        <v>1.5317453975404518</v>
+      </c>
+      <c r="S28" s="34">
         <f t="shared" si="2"/>
-        <v>1.5317453975404518</v>
-      </c>
-      <c r="S28" s="34">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1903,27 +1903,27 @@
         <v>1.2604719289064259</v>
       </c>
       <c r="F29" s="34">
-        <f>B$25*B22+B$26*C22+B$27*D22+B$28*E22+B$29*F22+B$30*G22</f>
+        <f t="shared" si="0"/>
         <v>1.2604719289064259</v>
       </c>
       <c r="H29" s="34">
-        <f>D29-F29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="O29" s="34">
         <v>1.2604719289064259</v>
       </c>
       <c r="Q29" s="34">
+        <f t="shared" si="4"/>
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="S29" s="34">
         <f t="shared" si="2"/>
-        <v>1.2604719289064259</v>
-      </c>
-      <c r="S29" s="34">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1935,27 +1935,27 @@
         <v>0.5</v>
       </c>
       <c r="F30" s="35">
-        <f>B$25*B23+B$26*C23+B$27*D23+B$28*E23+B$29*F23+B$30*G23</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="H30" s="35">
-        <f>D30-F30</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="O30" s="35">
         <v>0.5</v>
       </c>
       <c r="Q30" s="35">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="S30" s="35">
         <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="S30" s="35">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First steps towards error analysis code
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/DefocusQuadrupole.xlsx
+++ b/21-Spreads4Tests/DefocusQuadrupole.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethlong/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7F2DA9-76B8-8A4B-A3C9-BBDF46AF6D06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43C4D03-008F-5342-8A2E-31DFEFBB2B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27720" yWindow="500" windowWidth="29400" windowHeight="23120" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="4100" yWindow="640" windowWidth="26040" windowHeight="19000" activeTab="1" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Default" sheetId="1" r:id="rId1"/>
+    <sheet name="Shifted" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="44">
   <si>
     <t>p</t>
   </si>
@@ -291,6 +292,58 @@
   <si>
     <t>Deocus quad test sheet: no reference particle</t>
   </si>
+  <si>
+    <r>
+      <t>R'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>element</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Rprime</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>element</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <charset val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>r</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -299,7 +352,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -387,6 +440,20 @@
       <name val="Symbol"/>
       <charset val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -408,7 +475,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -570,11 +637,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -673,6 +785,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -990,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:S30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S30" sqref="A1:S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1973,4 +2094,1148 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA7ABC6-99A1-A148-B8F0-34F546E89C49}">
+  <dimension ref="A1:S44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39:O44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38"/>
+      <c r="L1" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="38"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="H2" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
+      <c r="L2" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="40"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="17"/>
+    </row>
+    <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="19">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="19">
+        <v>20</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>0.1</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="19">
+        <f>I10+B3</f>
+        <v>958.27208815999995</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4">
+        <f>E7</f>
+        <v>153.93033817521612</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="19">
+        <f>I10+M3</f>
+        <v>958.27208815999995</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="19">
+        <f>SQRT(B4^2 -I10^ 2)</f>
+        <v>194.75852619692921</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="9"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="24"/>
+      <c r="L5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="19">
+        <f>SQRT(M4^2 -I10^ 2)</f>
+        <v>194.75852619692921</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <f>B5/I10</f>
+        <v>0.20757148022900346</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f>B5*I13/1000</f>
+        <v>0.64964451573004278</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="H6" s="12"/>
+      <c r="J6" s="6"/>
+      <c r="L6" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6">
+        <f>M5/I10</f>
+        <v>0.20757148022900346</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <f>M12*I13/1000</f>
+        <v>1.6137238800416533</v>
+      </c>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <f>B5/B4</f>
+        <v>0.20323927682260837</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7">
+        <f>E4/E6</f>
+        <v>153.93033817521612</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1">
+        <f>I4*E6</f>
+        <v>100</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <f>M5/M4</f>
+        <v>0.20323927682260837</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7">
+        <f>P4/P6</f>
+        <v>61.968470093792504</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="9"/>
+      <c r="L8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="9"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
+      <c r="H10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="11">
+        <v>938.27208815999995</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="41"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11">
+        <f>B4+B5*B30</f>
+        <v>1055.6513512584645</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11">
+        <f>SQRT(1+(2*B30/B7) + B30^2)</f>
+        <v>2.4840106257623371</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="H11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="11">
+        <v>299792458</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11">
+        <f>M4+M5*B30</f>
+        <v>1055.6513512584645</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="19">
+        <f>SQRT(B11^2 -I10^ 2)</f>
+        <v>483.78224853098436</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12">
+        <f>SQRT(E7/E11)</f>
+        <v>7.8720054683538221</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12">
+        <f>1/I11</f>
+        <v>3.3356409519815204E-9</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="19">
+        <f>SQRT(M11^2 -I10^ 2)</f>
+        <v>483.78224853098436</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12">
+        <f>SQRT(P7/P11)</f>
+        <v>7.8720054683538239</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="30"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13">
+        <f>E12*E3</f>
+        <v>0.78720054683538221</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="H13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="8">
+        <f>I12*1000000000</f>
+        <v>3.3356409519815204</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="30"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13">
+        <f>P12*P3</f>
+        <v>0.78720054683538243</v>
+      </c>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="31"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="8">
+        <f>E12*E11</f>
+        <v>19.554145229450118</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="31"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="P14" s="8">
+        <f>P12*P11</f>
+        <v>7.8720054683538239</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="I17" s="49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3">
+        <f>COSH(E13)</f>
+        <v>1.326176919807601</v>
+      </c>
+      <c r="C18" s="4">
+        <f>SINH(E13)/E14</f>
+        <v>4.454604468864936E-2</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="34">
+        <v>0.2</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M18" s="3">
+        <f>COSH(P13)</f>
+        <v>1.3261769198076012</v>
+      </c>
+      <c r="N18" s="4">
+        <f>SINH(P13)/P14</f>
+        <v>0.11065284834228896</v>
+      </c>
+      <c r="O18" s="11">
+        <v>0</v>
+      </c>
+      <c r="P18" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="32">
+        <f>SINH(E13)*E14</f>
+        <v>17.032830365379439</v>
+      </c>
+      <c r="C19" s="9">
+        <f>COSH(E13)</f>
+        <v>1.326176919807601</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="I19" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="32">
+        <f>SINH(P13)*P14</f>
+        <v>6.8569877232920904</v>
+      </c>
+      <c r="N19" s="9">
+        <f>COSH(P13)</f>
+        <v>1.3261769198076012</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="12">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3">
+        <f>COS(E13)</f>
+        <v>0.70583115577702338</v>
+      </c>
+      <c r="E20" s="4">
+        <f>SIN(E13)/E14</f>
+        <v>3.622659549610921E-2</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="I20" s="35">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="3">
+        <f>COS(P13)</f>
+        <v>0.70583115577702327</v>
+      </c>
+      <c r="P20" s="4">
+        <f>SIN(P13)/P14</f>
+        <v>8.9987248147529314E-2</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="12">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="32">
+        <f>-SIN(E13)*E14</f>
+        <v>-13.851767538806278</v>
+      </c>
+      <c r="E21" s="9">
+        <f>COS(E13)</f>
+        <v>0.70583115577702338</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="12">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="32">
+        <f>-SIN(P13)*P14</f>
+        <v>-5.5763720956528555</v>
+      </c>
+      <c r="P21" s="9">
+        <f>COS(P13)</f>
+        <v>0.70583115577702327</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="12">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4">
+        <f>E3/B6^2</f>
+        <v>2.3209438578128516</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="12">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>1</v>
+      </c>
+      <c r="R22" s="4">
+        <f>P3/M6^2</f>
+        <v>2.3209438578128516</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="32">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+      <c r="F23" s="32">
+        <v>0</v>
+      </c>
+      <c r="G23" s="9">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="32">
+        <v>0</v>
+      </c>
+      <c r="N23" s="8">
+        <v>0</v>
+      </c>
+      <c r="O23" s="8">
+        <v>0</v>
+      </c>
+      <c r="P23" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="32">
+        <v>0</v>
+      </c>
+      <c r="R23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="33">
+        <f>B25-I18</f>
+        <v>0.3</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="33">
+        <f>B25</f>
+        <v>0.5</v>
+      </c>
+      <c r="N25" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" s="33">
+        <f>D25</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="46">
+        <v>0.1</v>
+      </c>
+      <c r="D26" s="34">
+        <f>B26</f>
+        <v>0.1</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="34">
+        <f t="shared" ref="M26:O30" si="0">B26</f>
+        <v>0.1</v>
+      </c>
+      <c r="O26" s="34">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="46">
+        <v>-0.3</v>
+      </c>
+      <c r="D27" s="34">
+        <f>B27-I19</f>
+        <v>-0.4</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="34">
+        <f t="shared" si="0"/>
+        <v>-0.3</v>
+      </c>
+      <c r="O27" s="34">
+        <f t="shared" si="0"/>
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="46">
+        <v>-0.2</v>
+      </c>
+      <c r="D28" s="34">
+        <f>B28</f>
+        <v>-0.2</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="34">
+        <f t="shared" si="0"/>
+        <v>-0.2</v>
+      </c>
+      <c r="O28" s="34">
+        <f t="shared" si="0"/>
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="46">
+        <v>0.1</v>
+      </c>
+      <c r="D29" s="34">
+        <f t="shared" ref="D29:D30" si="1">B29</f>
+        <v>0.1</v>
+      </c>
+      <c r="L29" s="1"/>
+      <c r="M29" s="34">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="O29" s="34">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="35">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="35">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="O30" s="35">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="18" x14ac:dyDescent="0.25">
+      <c r="C32" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="45">
+        <f t="array" ref="D32:D37">MMULT(B18:G23,D25:D30)</f>
+        <v>0.40230768041114523</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="45">
+        <f>D$25*B18+D$26*C18+D$27*D18+D$28*E18+D$29*F18+D$30*G18</f>
+        <v>0.40230768041114523</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H32" s="45">
+        <f t="shared" ref="H32:H37" si="2">D32-F32</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" s="45">
+        <f t="array" ref="O32:O37">MMULT(M18:R23,O25:O30)</f>
+        <v>0.40891836077650928</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q32" s="45">
+        <f>O$25*M18+O$26*N18+O$27*O18+O$28*P18+O$29*Q18+O$30*R18</f>
+        <v>0.40891836077650928</v>
+      </c>
+      <c r="R32" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="S32" s="45">
+        <f t="shared" ref="S32:S37" si="3">O32-Q32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D33" s="46">
+        <v>5.2424668015945919</v>
+      </c>
+      <c r="F33" s="46">
+        <f>D$25*B19+D$26*C19+D$27*D19+D$28*E19+D$29*F19+D$30*G19</f>
+        <v>5.2424668015945919</v>
+      </c>
+      <c r="H33" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O33" s="46">
+        <v>2.1897140089683869</v>
+      </c>
+      <c r="Q33" s="46">
+        <f>O$25*M19+O$26*N19+O$27*O19+O$28*P19+O$29*Q19+O$30*R19</f>
+        <v>2.1897140089683869</v>
+      </c>
+      <c r="S33" s="46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D34" s="46">
+        <v>-0.28957778141003121</v>
+      </c>
+      <c r="F34" s="46">
+        <f>D$25*B20+D$26*C20+D$27*D20+D$28*E20+D$29*F20+D$30*G20</f>
+        <v>-0.28957778141003121</v>
+      </c>
+      <c r="H34" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="46">
+        <v>-0.30032991194031522</v>
+      </c>
+      <c r="Q34" s="46">
+        <f>O$25*M20+O$26*N20+O$27*O20+O$28*P20+O$29*Q20+O$30*R20</f>
+        <v>-0.30032991194031522</v>
+      </c>
+      <c r="S34" s="46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D35" s="46">
+        <v>5.3995407843671073</v>
+      </c>
+      <c r="F35" s="46">
+        <f>D$25*B21+D$26*C21+D$27*D21+D$28*E21+D$29*F21+D$30*G21</f>
+        <v>5.3995407843671073</v>
+      </c>
+      <c r="H35" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="46">
+        <v>2.0893826071057378</v>
+      </c>
+      <c r="Q35" s="46">
+        <f>O$25*M21+O$26*N21+O$27*O21+O$28*P21+O$29*Q21+O$30*R21</f>
+        <v>2.0893826071057378</v>
+      </c>
+      <c r="S35" s="46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D36" s="46">
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="F36" s="46">
+        <f>D$25*B22+D$26*C22+D$27*D22+D$28*E22+D$29*F22+D$30*G22</f>
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="H36" s="46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="46">
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="Q36" s="46">
+        <f>O$25*M22+O$26*N22+O$27*O22+O$28*P22+O$29*Q22+O$30*R22</f>
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="S36" s="46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D37" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="F37" s="47">
+        <f>D$25*B23+D$26*C23+D$27*D23+D$28*E23+D$29*F23+D$30*G23</f>
+        <v>0.5</v>
+      </c>
+      <c r="H37" s="47">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O37" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="Q37" s="47">
+        <f>O$25*M23+O$26*N23+O$27*O23+O$28*P23+O$29*Q23+O$30*R23</f>
+        <v>0.5</v>
+      </c>
+      <c r="S37" s="47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C39" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="33">
+        <f>D32+I18</f>
+        <v>0.60230768041114524</v>
+      </c>
+      <c r="N39" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39" s="33">
+        <f>O32+I18</f>
+        <v>0.60891836077650929</v>
+      </c>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D40" s="34">
+        <f>D33</f>
+        <v>5.2424668015945919</v>
+      </c>
+      <c r="O40" s="34">
+        <f>O33</f>
+        <v>2.1897140089683869</v>
+      </c>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D41" s="34">
+        <f>D34+I19</f>
+        <v>-0.1895777814100312</v>
+      </c>
+      <c r="O41" s="34">
+        <f>O34+I19</f>
+        <v>-0.20032991194031521</v>
+      </c>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D42" s="34">
+        <f>D35</f>
+        <v>5.3995407843671073</v>
+      </c>
+      <c r="O42" s="34">
+        <f>O35</f>
+        <v>2.0893826071057378</v>
+      </c>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D43" s="34">
+        <f>D36</f>
+        <v>1.2604719289064259</v>
+      </c>
+      <c r="O43" s="34">
+        <f t="shared" ref="O43:O44" si="4">O36</f>
+        <v>1.2604719289064259</v>
+      </c>
+    </row>
+    <row r="44" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="D44" s="35">
+        <f>D37</f>
+        <v>0.5</v>
+      </c>
+      <c r="O44" s="35">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>